<commit_message>
Back to the purgatory
</commit_message>
<xml_diff>
--- a/Excel/Data/Projektek_Épületek_Kapcsolótábla.xlsx
+++ b/Excel/Data/Projektek_Épületek_Kapcsolótábla.xlsx
@@ -36,12 +36,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFE0E0E0" tint="0"/>
+      <color rgb="FF000000" tint="0"/>
       <name val="Calibri"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFE0E0E0" tint="0"/>
+      <color rgb="FF000000" tint="0"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -65,15 +65,15 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF202020"/>
-        <bgColor rgb="FF202020"/>
+      <patternFill patternType="none">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF202020"/>
-        <bgColor rgb="FF202020"/>
+      <patternFill patternType="none">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -435,7 +435,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="C5" sqref="C5"/>
@@ -443,7 +443,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="true" min="1" max="1" width="14.0625"/>
+    <col customWidth="true" min="1" max="1" width="13.8359375"/>
     <col customWidth="true" min="2" max="2" width="22.55859375"/>
     <col customWidth="true" min="3" max="3" width="22.703125"/>
   </cols>
@@ -542,6 +542,61 @@
         <v>24</v>
       </c>
     </row>
+    <row outlineLevel="0" r="9">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4">
+        <v>6</v>
+      </c>
+      <c r="C9" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="10">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4">
+        <v>7</v>
+      </c>
+      <c r="C10" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="11">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4">
+        <v>7</v>
+      </c>
+      <c r="C11" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="12">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4">
+        <v>7</v>
+      </c>
+      <c r="C12" s="4">
+        <v>14</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="13">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4">
+        <v>7</v>
+      </c>
+      <c r="C13" s="4">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>